<commit_message>
atualizacao da programacao da disciplina
</commit_message>
<xml_diff>
--- a/projeto_final.xlsx
+++ b/projeto_final.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
   <si>
     <t>Tema</t>
   </si>
@@ -61,6 +61,30 @@
   </si>
   <si>
     <t xml:space="preserve">Ricardo Ribeiro</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ambiente CyberBattlesim com Reinforcement Learning</t>
+  </si>
+  <si>
+    <t>Davi</t>
+  </si>
+  <si>
+    <t>Henrique</t>
+  </si>
+  <si>
+    <t>Luiza</t>
+  </si>
+  <si>
+    <t>Nicolas</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Markov Decision Process no ambiente SimpleGrid do Gymnasium</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ana Carolina</t>
+  </si>
+  <si>
+    <t>entregue</t>
   </si>
 </sst>
 </file>
@@ -767,42 +791,66 @@
       <c r="E7" s="5"/>
       <c r="F7" s="5"/>
     </row>
-    <row r="8" ht="14.25">
-      <c r="A8" s="5"/>
-      <c r="B8" s="5"/>
-      <c r="C8" s="5"/>
+    <row r="8" ht="28.5">
+      <c r="A8" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="C8" s="6" t="s">
+        <v>12</v>
+      </c>
       <c r="D8" s="5"/>
       <c r="E8" s="5"/>
       <c r="F8" s="5"/>
     </row>
     <row r="9" ht="14.25">
       <c r="A9" s="5"/>
-      <c r="B9" s="5"/>
-      <c r="C9" s="5"/>
+      <c r="B9" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="C9" s="6" t="s">
+        <v>12</v>
+      </c>
       <c r="D9" s="5"/>
       <c r="E9" s="5"/>
       <c r="F9" s="5"/>
     </row>
     <row r="10" ht="14.25">
       <c r="A10" s="5"/>
-      <c r="B10" s="5"/>
-      <c r="C10" s="5"/>
+      <c r="B10" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="C10" s="6" t="s">
+        <v>12</v>
+      </c>
       <c r="D10" s="5"/>
       <c r="E10" s="5"/>
       <c r="F10" s="5"/>
     </row>
     <row r="11" ht="14.25">
       <c r="A11" s="5"/>
-      <c r="B11" s="5"/>
-      <c r="C11" s="5"/>
+      <c r="B11" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="C11" s="6" t="s">
+        <v>12</v>
+      </c>
       <c r="D11" s="5"/>
       <c r="E11" s="5"/>
       <c r="F11" s="5"/>
     </row>
-    <row r="12" ht="14.25">
-      <c r="A12" s="5"/>
-      <c r="B12" s="5"/>
-      <c r="C12" s="5"/>
+    <row r="12" ht="42.75">
+      <c r="A12" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="B12" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="C12" s="6" t="s">
+        <v>23</v>
+      </c>
       <c r="D12" s="5"/>
       <c r="E12" s="5"/>
       <c r="F12" s="5"/>

</xml_diff>